<commit_message>
made changes to AdDetails file and uploaded image using yaml file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/PragraAdvertisement.xlsx
+++ b/src/test/resources/testdata/PragraAdvertisement.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="QA" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="BA" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Title</t>
   </si>
@@ -20,6 +21,68 @@
   </si>
   <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Certified Business Analysis Professional 
+(CBAP®) Certification Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our Certified Business Analysis program led by the industry’s expert with 12 Years of immerse experience, 
+students learn fundamentals to integrate appropriate technologies for analysis and development of business processes.
+**** No IT Background required, start your first job in IT****
+***  Free Demo class on Saturday from 3 PM to 5 PM ***
+**   Batch starts in Nov, 2018 in Mississauga  **
+*    LIMITED SEATS *
+Pragra is providing quick and detailed course for trending career option “Business Analyst”. Course encircles complete understanding of Business
+Analysis- no matter which back ground you from. Here, we provide fully job-oriented training with the simulation of the real work environment.
+We promise to support you and push you to learn, grow and become what you’ve always wanted to be.
+WHY THIS PROGRAM
+IT is one of the fastest growing careers in today’s economy. PRAGRA programs were designed to help learners develop the skills and professional
+network needed to capitalize on the demand for 182,000 ICT workers in Canada by 2019, with ICTC predicting that the most in-demand roles will 
+include Business Analyst, Software Developers Scrum Master, Agile team Lead.
+FEATURES
+&gt; Pass the IIBA-CBAP® exam and Understand Business Analysis Key Concepts
+&gt; Understand the Business Analysis Core Concept Model
+&gt; As per knowledge areas of BABOK® Guide Version 3
+&gt; Case Studies: allow you to explore practical situations in a structured learning environment.
+&gt; Industry Project: As part of a small consulting team, you'll tackle a real business problem with a client company.
+&gt; Guide practices related to 30 business analysis tasks in six knowledge areas
+&gt; Understand 50 business analysis tools and techniques
+&gt; Understand the five business analysis perspectives: Agile, Business Intelligence, Information Technology, Business Architecture and Business 
+Process Management
+&gt; Setup and handle projects on a JIRA cloud site
+&gt; Apply best practices crucial for getting the maximum value from the Scrum methodology
+&gt; Create sound business arguments, using financial and cost analysis to justify any process change.
+LINK: https://pragra.co/learning/business-analysis
+BENEFITS
+Benefit from a wide range of career services to position you for success through graduation and beyond. Part Time Study, weekend in person + weekday 
+online classes, while maintaining your work schedule.
+The Agile Scrum Master certification course is best suited for:
+&gt; Team Leaders
+&gt; Aspiring business analysts with over seven to ten years of experience
+&gt; Senior Analysis Professionals and Project Managers
+&gt; Members of Scrum teams such as developers, Scrum Masters, and product owners
+&gt; Teams transitioning to Scrum
+CAREER SERVICES
+Co-Op Trainings and Certification, Resume Creation and highlighting your skills. Creation of portfolio of Business Analyst to showcase your knowledge. 
+**The material covered in this program is subject to change due to market demand.
+ASPECTS
+&gt; Study part-time, three days a week, while maintaining your work schedule.
+&gt; Benefit from a wide range of career services to position you for success through program completion and beyond.
+&gt; Develop UML, tables and presentation slides that present findings in a compelling manner.
+&gt; Prepare formal reports that communicate key findings and recommendations to decision makers.
+&gt; We refund your fees if you think program was not worth to attend at the end of month. 
+DURATION: 8 Weeks training. 
+INFO:
+This program is offered by highly qualified consultants of PRAGRA: 
+https://www.pragra.co, Contact the team for detailed curriculum at: +1 (416) 910-8340, +1 (647)-343-5453, info@pragra.co
+Keywords: IT Jobs, Jobs, IT trainings, IT Training, Computer training Programs, Free programs, Free training , Free Learning, BA Jobs, BA Training, CBAP
+certification, Agile Training , Free Agile Training, Business Analyst Jobs, PMP Certification, PMP, Project Management Professional, Project Management
+Training, Project Management Institute, PMI, CAPM Certification, BA Training, Business Analysis Certification, Business Analysis, CBAP, Certified Business
+Analysis Professional, CCBA Training, CBAP Certification, IIBA, International Institute of Business Analysis, Mississauga PMP Training, Brampton PMP
+Training, Toronto PMP Training, Mississauga CBAP Training, Brampton CBAP Training, Toronto CBAP Training, Business Analysis Training, Pragra PMP 
+Training, Pragra CBAP Training, Pragra Business Analysis Training
+</t>
   </si>
   <si>
     <t xml:space="preserve">Start Your IT Career as QA Automation Engineer </t>
@@ -55,6 +118,9 @@
   <si>
     <t xml:space="preserve"> L5M</t>
   </si>
+  <si>
+    <t>L6S</t>
+  </si>
 </sst>
 </file>
 
@@ -89,12 +155,18 @@
       <name val="Larsseit"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor rgb="FFBDD6EE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -121,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -129,15 +201,18 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -147,6 +222,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -177,18 +256,59 @@
       </c>
     </row>
     <row r="2" ht="341.25" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="6"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="38.29"/>
+    <col customWidth="1" min="2" max="2" width="131.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" s="5"/>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Adding code for reading multiple sheets from static excel reader class
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/PragraAdvertisement.xlsx
+++ b/src/test/resources/testdata/PragraAdvertisement.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="QA" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="BA" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="DevOps" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Title</t>
   </si>
@@ -20,11 +21,54 @@
     <t>Description</t>
   </si>
   <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Start your career in DevOps/IT</t>
+  </si>
+  <si>
+    <t>Our program will provide you a kick start for your career as DevOps Engineer, the domain which is capturing market so quickly and 
+fixing the gap between developer and operational engineer. This training covers fundamentals, including managing group settings 
+and customizing tasks, to more in-depth material such as deploying a private cloud. If you aspire to be a DevOps Engineer or want
+ to expand your existing skill set, this is the training for you. You will master configuration management; continuous integration 
+deployment, delivery and monitoring using DevOps tools such as Git, Docker, Jenkins, Puppet and Nagios in a practical, hands on 
+and interactive approach. 
+*** Self Paced Training with Assignments and Project Hands-On ***
+*** Free Demo class on Sunday from 10 AM to 2 PM ***
+*** Batch starts in November 2018 in Mississauga *** 
+*** Get Certified with Lifetime Access *** 
+*** Job Assistance with Career Services *** 
+DURATION: 12 Weeks training. 
+Build Tools: Maven CI 
+Testing : JUnit 
+Version Management: GIT Configuration 
+Tools: Docker, Minikube, Chef, Puppet, Ansible 
+ASPECTS 
+&gt; Study part-time, two days a week, while maintaining your work schedule.
+&gt; Program tailored for people who are new to IT field or want to progress towards DevOps. 
+&gt; Benefit from a wide range of career services to position you for success through program completion and beyond. 
+CAREER SERVICES 
+&gt; Co-Op Trainings and Certification, Resume Creation and highlighting your skills.
+&gt; Creation of portfolio of DevOps Engineer to showcase your knowledge. 
+ROADMAP 
+&gt; After successful completion of this workshop one will continue further with professional program advance their knowledge. 
+&gt; These courses act as foundation for the students who like to pursue their career in cloud IT or DevOps field.
+INFO: This program is offered by highly qualified consultants of PRAGRA: https://www.pragra.co, Contact the team for detailed curriculum at: (647)-343-5453, info@pragra.co 
+Keywords: DevOps Jobs, Dev Ops, Ansible, Infra Jobs, IT Jobs, QA Jobs , Computer Jobs, Technician, Network Engineer, Engineering Jobs, Sysadmin, DevOps engineer 
+TRANSFORM CAREER TRANSFORM LIFE</t>
+  </si>
+  <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>L5M</t>
   </si>
   <si>
     <t>Certified Business Analysis Professional 
 (CBAP®) Certification Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Your IT Career as QA Automation Engineer </t>
   </si>
   <si>
     <t xml:space="preserve">Our Certified Business Analysis program led by the industry’s expert with 12 Years of immerse experience, 
@@ -85,7 +129,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Start Your IT Career as QA Automation Engineer </t>
+    <t>L6S</t>
   </si>
   <si>
     <t>**** No IT Background required, start your first job in IT*** 
@@ -117,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve"> L5M</t>
-  </si>
-  <si>
-    <t>L6S</t>
   </si>
 </sst>
 </file>
@@ -229,6 +270,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -252,18 +297,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" ht="341.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -296,18 +341,59 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="29.14"/>
+    <col customWidth="1" min="2" max="2" width="113.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>